<commit_message>
Atualizado por script em 09-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/costa-rica_primera-division_2023-2024.xlsx
+++ b/2023/costa-rica_primera-division_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V111"/>
+  <dimension ref="A1:V113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10669,6 +10669,190 @@
         </is>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>costa-rica</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>45239.13541666666</v>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Puntarenas FC</t>
+        </is>
+      </c>
+      <c r="G112" t="n">
+        <v>4</v>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Sporting San Jose</t>
+        </is>
+      </c>
+      <c r="I112" t="n">
+        <v>0</v>
+      </c>
+      <c r="J112" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>05/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="L112" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>09/11/2023 03:11</t>
+        </is>
+      </c>
+      <c r="N112" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>05/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P112" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>09/11/2023 03:11</t>
+        </is>
+      </c>
+      <c r="R112" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>05/11/2023 00:12</t>
+        </is>
+      </c>
+      <c r="T112" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>09/11/2023 03:11</t>
+        </is>
+      </c>
+      <c r="V112" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/puntarenas-fc-sporting-san-jose/UcDN9TAH/</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>costa-rica</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>45239.14583333334</v>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Herediano</t>
+        </is>
+      </c>
+      <c r="G113" t="n">
+        <v>1</v>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Cartagines</t>
+        </is>
+      </c>
+      <c r="I113" t="n">
+        <v>0</v>
+      </c>
+      <c r="J113" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>05/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="L113" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>09/11/2023 03:21</t>
+        </is>
+      </c>
+      <c r="N113" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>05/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P113" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>09/11/2023 03:21</t>
+        </is>
+      </c>
+      <c r="R113" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>05/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T113" t="n">
+        <v>4.92</v>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>09/11/2023 03:21</t>
+        </is>
+      </c>
+      <c r="V113" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/herediano-cartagines/tO17DBBh/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 10-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/costa-rica_primera-division_2023-2024.xlsx
+++ b/2023/costa-rica_primera-division_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V113"/>
+  <dimension ref="A1:V114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9129,7 +9129,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>AD Santos</t>
+          <t>Grecia</t>
         </is>
       </c>
       <c r="G95" t="n">
@@ -9137,14 +9137,14 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Zeledon</t>
+          <t>Liberia</t>
         </is>
       </c>
       <c r="I95" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J95" t="n">
-        <v>1.88</v>
+        <v>2.71</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -9152,48 +9152,48 @@
         </is>
       </c>
       <c r="L95" t="n">
-        <v>1.97</v>
+        <v>2.39</v>
       </c>
       <c r="M95" t="inlineStr">
         <is>
+          <t>22/10/2023 23:51</t>
+        </is>
+      </c>
+      <c r="N95" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>19/10/2023 18:43</t>
+        </is>
+      </c>
+      <c r="P95" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
           <t>22/10/2023 23:50</t>
         </is>
       </c>
-      <c r="N95" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="O95" t="inlineStr">
+      <c r="R95" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="S95" t="inlineStr">
         <is>
           <t>19/10/2023 18:43</t>
         </is>
       </c>
-      <c r="P95" t="n">
-        <v>3.52</v>
-      </c>
-      <c r="Q95" t="inlineStr">
-        <is>
-          <t>22/10/2023 23:50</t>
-        </is>
-      </c>
-      <c r="R95" t="n">
-        <v>4.06</v>
-      </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>19/10/2023 18:43</t>
-        </is>
-      </c>
       <c r="T95" t="n">
-        <v>3.95</v>
+        <v>2.87</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>22/10/2023 23:50</t>
+          <t>22/10/2023 23:51</t>
         </is>
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/costa-rica/primera-division/santos-de-guapiles-zeledon/Sb0cnZCg/</t>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/grecia-liberia/0lhAqXdC/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Grecia</t>
+          <t>AD Santos</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,14 +9229,14 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Liberia</t>
+          <t>Zeledon</t>
         </is>
       </c>
       <c r="I96" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>2.71</v>
+        <v>1.88</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -9244,15 +9244,15 @@
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.39</v>
+        <v>1.97</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>22/10/2023 23:51</t>
+          <t>22/10/2023 23:50</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.38</v>
+        <v>3.6</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -9260,7 +9260,7 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.6</v>
+        <v>3.52</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,7 +9268,7 @@
         </is>
       </c>
       <c r="R96" t="n">
-        <v>2.57</v>
+        <v>4.06</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
@@ -9276,16 +9276,16 @@
         </is>
       </c>
       <c r="T96" t="n">
-        <v>2.87</v>
+        <v>3.95</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>22/10/2023 23:51</t>
+          <t>22/10/2023 23:50</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/costa-rica/primera-division/grecia-liberia/0lhAqXdC/</t>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/santos-de-guapiles-zeledon/Sb0cnZCg/</t>
         </is>
       </c>
     </row>
@@ -10850,6 +10850,98 @@
       <c r="V113" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/costa-rica/primera-division/herediano-cartagines/tO17DBBh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>costa-rica</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>45240.125</v>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Liberia</t>
+        </is>
+      </c>
+      <c r="G114" t="n">
+        <v>1</v>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Saprissa</t>
+        </is>
+      </c>
+      <c r="I114" t="n">
+        <v>2</v>
+      </c>
+      <c r="J114" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>05/11/2023 18:13</t>
+        </is>
+      </c>
+      <c r="L114" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>10/11/2023 02:58</t>
+        </is>
+      </c>
+      <c r="N114" t="n">
+        <v>3.97</v>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>05/11/2023 18:13</t>
+        </is>
+      </c>
+      <c r="P114" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>10/11/2023 02:58</t>
+        </is>
+      </c>
+      <c r="R114" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>05/11/2023 18:13</t>
+        </is>
+      </c>
+      <c r="T114" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>10/11/2023 02:58</t>
+        </is>
+      </c>
+      <c r="V114" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/liberia-saprissa/YVJEBkt5/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 17-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/costa-rica_primera-division_2023-2024.xlsx
+++ b/2023/costa-rica_primera-division_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V120"/>
+  <dimension ref="A1:V121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10509,71 +10509,71 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Alajuelense</t>
+          <t>AD Santos</t>
         </is>
       </c>
       <c r="G110" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>San Carlos</t>
+        </is>
+      </c>
+      <c r="I110" t="n">
         <v>2</v>
       </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>Grecia</t>
-        </is>
-      </c>
-      <c r="I110" t="n">
-        <v>0</v>
-      </c>
       <c r="J110" t="n">
-        <v>1.19</v>
+        <v>2.57</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>05/11/2023 22:12</t>
+          <t>04/11/2023 22:12</t>
         </is>
       </c>
       <c r="L110" t="n">
-        <v>1.25</v>
+        <v>2.51</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
+          <t>09/11/2023 00:59</t>
+        </is>
+      </c>
+      <c r="N110" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>04/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P110" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
           <t>09/11/2023 00:56</t>
         </is>
       </c>
-      <c r="N110" t="n">
-        <v>7.28</v>
-      </c>
-      <c r="O110" t="inlineStr">
-        <is>
-          <t>05/11/2023 22:12</t>
-        </is>
-      </c>
-      <c r="P110" t="n">
-        <v>6.33</v>
-      </c>
-      <c r="Q110" t="inlineStr">
-        <is>
-          <t>09/11/2023 00:57</t>
-        </is>
-      </c>
       <c r="R110" t="n">
-        <v>12.63</v>
+        <v>2.78</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>05/11/2023 22:12</t>
+          <t>04/11/2023 22:12</t>
         </is>
       </c>
       <c r="T110" t="n">
-        <v>9.99</v>
+        <v>2.87</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>09/11/2023 00:57</t>
+          <t>09/11/2023 00:59</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/costa-rica/primera-division/alajuelense-grecia/v9KACVQb/</t>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/santos-de-guapiles-san-carlos/baC2Eidn/</t>
         </is>
       </c>
     </row>
@@ -10601,71 +10601,71 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>AD Santos</t>
+          <t>Alajuelense</t>
         </is>
       </c>
       <c r="G111" t="n">
+        <v>2</v>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Grecia</t>
+        </is>
+      </c>
+      <c r="I111" t="n">
         <v>0</v>
       </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>San Carlos</t>
-        </is>
-      </c>
-      <c r="I111" t="n">
-        <v>2</v>
-      </c>
       <c r="J111" t="n">
-        <v>2.57</v>
+        <v>1.19</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>04/11/2023 22:12</t>
+          <t>05/11/2023 22:12</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>2.51</v>
+        <v>1.25</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>09/11/2023 00:59</t>
+          <t>09/11/2023 00:56</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>3.39</v>
+        <v>7.28</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>04/11/2023 22:12</t>
+          <t>05/11/2023 22:12</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>3.37</v>
+        <v>6.33</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>09/11/2023 00:56</t>
+          <t>09/11/2023 00:57</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.78</v>
+        <v>12.63</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>04/11/2023 22:12</t>
+          <t>05/11/2023 22:12</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.87</v>
+        <v>9.99</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>09/11/2023 00:59</t>
+          <t>09/11/2023 00:57</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/costa-rica/primera-division/santos-de-guapiles-san-carlos/baC2Eidn/</t>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/alajuelense-grecia/v9KACVQb/</t>
         </is>
       </c>
     </row>
@@ -11494,6 +11494,98 @@
       <c r="V120" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/costa-rica/primera-division/sporting-san-jose-santos-de-guapiles/29GkD2H9/</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>costa-rica</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>45245.91666666666</v>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Guanacasteca</t>
+        </is>
+      </c>
+      <c r="G121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Herediano</t>
+        </is>
+      </c>
+      <c r="I121" t="n">
+        <v>1</v>
+      </c>
+      <c r="J121" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:57</t>
+        </is>
+      </c>
+      <c r="L121" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:57</t>
+        </is>
+      </c>
+      <c r="N121" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:57</t>
+        </is>
+      </c>
+      <c r="P121" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:57</t>
+        </is>
+      </c>
+      <c r="R121" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:57</t>
+        </is>
+      </c>
+      <c r="T121" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="U121" t="inlineStr">
+        <is>
+          <t>18/10/2023 22:57</t>
+        </is>
+      </c>
+      <c r="V121" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/guanacasteca-herediano/QVwSWgD6/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 22-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/costa-rica_primera-division_2023-2024.xlsx
+++ b/2023/costa-rica_primera-division_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V121"/>
+  <dimension ref="A1:V122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9129,7 +9129,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>AD Santos</t>
+          <t>Grecia</t>
         </is>
       </c>
       <c r="G95" t="n">
@@ -9137,14 +9137,14 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Zeledon</t>
+          <t>Liberia</t>
         </is>
       </c>
       <c r="I95" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J95" t="n">
-        <v>1.88</v>
+        <v>2.71</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -9152,48 +9152,48 @@
         </is>
       </c>
       <c r="L95" t="n">
-        <v>1.97</v>
+        <v>2.39</v>
       </c>
       <c r="M95" t="inlineStr">
         <is>
+          <t>22/10/2023 23:51</t>
+        </is>
+      </c>
+      <c r="N95" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>19/10/2023 18:43</t>
+        </is>
+      </c>
+      <c r="P95" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
           <t>22/10/2023 23:50</t>
         </is>
       </c>
-      <c r="N95" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="O95" t="inlineStr">
+      <c r="R95" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="S95" t="inlineStr">
         <is>
           <t>19/10/2023 18:43</t>
         </is>
       </c>
-      <c r="P95" t="n">
-        <v>3.52</v>
-      </c>
-      <c r="Q95" t="inlineStr">
-        <is>
-          <t>22/10/2023 23:50</t>
-        </is>
-      </c>
-      <c r="R95" t="n">
-        <v>4.06</v>
-      </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>19/10/2023 18:43</t>
-        </is>
-      </c>
       <c r="T95" t="n">
-        <v>3.95</v>
+        <v>2.87</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>22/10/2023 23:50</t>
+          <t>22/10/2023 23:51</t>
         </is>
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/costa-rica/primera-division/santos-de-guapiles-zeledon/Sb0cnZCg/</t>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/grecia-liberia/0lhAqXdC/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Grecia</t>
+          <t>AD Santos</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,14 +9229,14 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Liberia</t>
+          <t>Zeledon</t>
         </is>
       </c>
       <c r="I96" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>2.71</v>
+        <v>1.88</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -9244,15 +9244,15 @@
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.39</v>
+        <v>1.97</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>22/10/2023 23:51</t>
+          <t>22/10/2023 23:50</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.38</v>
+        <v>3.6</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -9260,7 +9260,7 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.6</v>
+        <v>3.52</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
@@ -9268,7 +9268,7 @@
         </is>
       </c>
       <c r="R96" t="n">
-        <v>2.57</v>
+        <v>4.06</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
@@ -9276,16 +9276,16 @@
         </is>
       </c>
       <c r="T96" t="n">
-        <v>2.87</v>
+        <v>3.95</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>22/10/2023 23:51</t>
+          <t>22/10/2023 23:50</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/costa-rica/primera-division/grecia-liberia/0lhAqXdC/</t>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/santos-de-guapiles-zeledon/Sb0cnZCg/</t>
         </is>
       </c>
     </row>
@@ -11586,6 +11586,98 @@
       <c r="V121" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/costa-rica/primera-division/guanacasteca-herediano/QVwSWgD6/</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>costa-rica</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>45252.125</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Sporting San Jose</t>
+        </is>
+      </c>
+      <c r="G122" t="n">
+        <v>1</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Cartagines</t>
+        </is>
+      </c>
+      <c r="I122" t="n">
+        <v>1</v>
+      </c>
+      <c r="J122" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>15/11/2023 05:12</t>
+        </is>
+      </c>
+      <c r="L122" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>21/11/2023 22:48</t>
+        </is>
+      </c>
+      <c r="N122" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>15/11/2023 05:12</t>
+        </is>
+      </c>
+      <c r="P122" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>21/11/2023 22:48</t>
+        </is>
+      </c>
+      <c r="R122" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>15/11/2023 05:12</t>
+        </is>
+      </c>
+      <c r="T122" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
+          <t>21/11/2023 22:48</t>
+        </is>
+      </c>
+      <c r="V122" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/costa-rica/primera-division/sporting-san-jose-cartagines/jZlw4bvd/</t>
         </is>
       </c>
     </row>

</xml_diff>